<commit_message>
Ajustes finais da arvore
</commit_message>
<xml_diff>
--- a/tabelaAnalise.xlsx
+++ b/tabelaAnalise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vbsni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Vinício\UFU\7\CC\analisador-sintatico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC001D0F-D526-487C-A63D-439DE2420DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630CE741-6ED0-4E34-BE12-81905D5B4C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,7 +343,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -663,7 +663,7 @@
   <dimension ref="A1:AH35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,55 +1023,55 @@
         <v>4</v>
       </c>
       <c r="N4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="X4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AD4" s="9">
         <v>4</v>
-      </c>
-      <c r="O4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="P4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="R4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="T4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="U4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="V4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="W4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="X4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AD4" s="9">
-        <v>-1</v>
       </c>
       <c r="AE4" s="1">
         <v>-1</v>
@@ -2756,6 +2756,7 @@
       <c r="AF24" s="7"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AB25" s="8"/>
       <c r="AE25" s="7"/>
       <c r="AF25" s="7"/>
     </row>

</xml_diff>